<commit_message>
updated the file lists
</commit_message>
<xml_diff>
--- a/data/577 Projects/2010-2011/file list.xlsx
+++ b/data/577 Projects/2010-2011/file list.xlsx
@@ -37,7 +37,7 @@
     <t>~\577 projects\fall2015\projects\team01\team01b\Development\RCP</t>
   </si>
   <si>
-    <t>Example.</t>
+    <t>This is an exampke for the things to fill. The URL should be point to the folder where the LCP, SSAD, OCD are found.</t>
   </si>
 </sst>
 </file>
@@ -411,13 +411,13 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="4" max="4" width="55.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>